<commit_message>
replaced m_fire with smoke_data
</commit_message>
<xml_diff>
--- a/Calibration/Asthma states/CHARM 5 to 3 state calibration - 30may2023.xlsx
+++ b/Calibration/Asthma states/CHARM 5 to 3 state calibration - 30may2023.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\smaya\Box\AA_Sigal_Documents\Climate - Health\Modeling\Calibration\Asthma states\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26699D22-BC56-4761-A1EE-0E0259B0DB0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F3E95AE-99FE-496D-BBB6-634D4592F705}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-1995" windowWidth="29040" windowHeight="17640" activeTab="2" xr2:uid="{95115A8E-B4AD-A141-83E3-2764AA2AD3E5}"/>
   </bookViews>
@@ -260,7 +260,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="81">
   <si>
     <t>calculated based on 1-5 values + co-distrib</t>
   </si>
@@ -361,9 +361,6 @@
     <t xml:space="preserve">To obtain the co-distribution of prevalence, we followed the example set in Soler et al (2019). Their study aimed to validate the Asthma Control Test (ACT) questionnaire, and compared ACT scores to physician global assessment scores for a sample of smoking asthmatics. </t>
   </si>
   <si>
-    <t>Model @ Equilibrium</t>
-  </si>
-  <si>
     <t>target 3-way prevalence @ Equilibrium</t>
   </si>
   <si>
@@ -475,21 +472,12 @@
     <t>2-weekly probs</t>
   </si>
   <si>
-    <t>If Week 0 = all somewhat controlled</t>
-  </si>
-  <si>
-    <t>CONVERT TO RATES</t>
-  </si>
-  <si>
     <t xml:space="preserve">t for 2-wk = </t>
   </si>
   <si>
     <t xml:space="preserve">t for 1-wk = </t>
   </si>
   <si>
-    <t>THEN BACK TO PROBS</t>
-  </si>
-  <si>
     <t>…</t>
   </si>
   <si>
@@ -497,6 +485,24 @@
   </si>
   <si>
     <t>Delta from s-s</t>
+  </si>
+  <si>
+    <t>Modeled prevalence at steady-state</t>
+  </si>
+  <si>
+    <t>Model @ Equilibrium using 2-week probs</t>
+  </si>
+  <si>
+    <t>Model @ Equilibrium using 1-week probs</t>
+  </si>
+  <si>
+    <t>Delta vs. Lit</t>
+  </si>
+  <si>
+    <t>THEN BACK TO 1-week PROBS</t>
+  </si>
+  <si>
+    <t>CONVERT TO RATES 2 weekly</t>
   </si>
 </sst>
 </file>
@@ -508,9 +514,16 @@
     <numFmt numFmtId="165" formatCode="0.000"/>
     <numFmt numFmtId="166" formatCode="0.00000"/>
   </numFmts>
-  <fonts count="16" x14ac:knownFonts="1">
+  <fonts count="17" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -819,9 +832,9 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="123">
+  <cellXfs count="125">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -829,7 +842,7 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
@@ -862,332 +875,338 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="15" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="5" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="5" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="5" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="5" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="5" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="5" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="5" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="5" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="15" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="13" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="12" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="12" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="13" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="12" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="13" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="13" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="12" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="12" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="13" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="12" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="13" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="12" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="11" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="11" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="12" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="11" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="12" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="12" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="11" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="11" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="12" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="11" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="12" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1637,8 +1656,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9454E13-E3C1-3E46-8368-D2DB362951ED}">
   <dimension ref="B1:P32"/>
   <sheetViews>
-    <sheetView topLeftCell="H4" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="L11" sqref="L11:L15"/>
+    <sheetView topLeftCell="A5" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="P11" sqref="P11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.83203125" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -1704,7 +1723,7 @@
     </row>
     <row r="5" spans="2:16" x14ac:dyDescent="0.35">
       <c r="C5" s="13" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D5" s="31">
         <v>0.23300000000000001</v>
@@ -1792,46 +1811,46 @@
       <c r="G8" s="2"/>
     </row>
     <row r="9" spans="2:16" x14ac:dyDescent="0.35">
-      <c r="D9" s="98" t="s">
+      <c r="D9" s="114" t="s">
         <v>7</v>
       </c>
-      <c r="E9" s="99"/>
-      <c r="F9" s="99"/>
-      <c r="G9" s="99"/>
-      <c r="H9" s="99"/>
-      <c r="I9" s="99"/>
-      <c r="J9" s="99"/>
-      <c r="K9" s="100"/>
-      <c r="L9" s="101" t="s">
-        <v>35</v>
-      </c>
-      <c r="M9" s="102"/>
-      <c r="N9" s="102"/>
-      <c r="O9" s="103"/>
-      <c r="P9" s="103"/>
-    </row>
-    <row r="10" spans="2:16" ht="31" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E9" s="115"/>
+      <c r="F9" s="115"/>
+      <c r="G9" s="115"/>
+      <c r="H9" s="115"/>
+      <c r="I9" s="115"/>
+      <c r="J9" s="115"/>
+      <c r="K9" s="116"/>
+      <c r="L9" s="117" t="s">
+        <v>34</v>
+      </c>
+      <c r="M9" s="118"/>
+      <c r="N9" s="118"/>
+      <c r="O9" s="119"/>
+      <c r="P9" s="119"/>
+    </row>
+    <row r="10" spans="2:16" ht="67" customHeight="1" x14ac:dyDescent="0.35">
       <c r="D10" s="17" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G10" s="2"/>
       <c r="I10" s="17" t="s">
         <v>3</v>
       </c>
       <c r="L10" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="M10" s="28" t="s">
-        <v>33</v>
+        <v>76</v>
       </c>
       <c r="N10" s="15" t="s">
+        <v>78</v>
+      </c>
+      <c r="O10" s="28" t="s">
+        <v>77</v>
+      </c>
+      <c r="P10" s="15" t="s">
         <v>37</v>
-      </c>
-      <c r="O10" s="28" t="s">
-        <v>71</v>
-      </c>
-      <c r="P10" s="15" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="11" spans="2:16" x14ac:dyDescent="0.35">
@@ -1869,12 +1888,11 @@
         <v>-2.0166666666666666E-2</v>
       </c>
       <c r="O11" s="37">
-        <f>'Check-calib2transprob'!N26</f>
-        <v>6.0994204574805484E-2</v>
+        <v>5.586E-2</v>
       </c>
       <c r="P11" s="30">
         <f>O11-L11</f>
-        <v>2.2160871241472153E-2</v>
+        <v>1.7026666666666669E-2</v>
       </c>
     </row>
     <row r="12" spans="2:16" x14ac:dyDescent="0.35">
@@ -1915,12 +1933,11 @@
         <v>3.1666666666666787E-3</v>
       </c>
       <c r="O12" s="37">
-        <f>'Check-calib2transprob'!M26</f>
-        <v>0.19573181473487794</v>
+        <v>0.19672999999999999</v>
       </c>
       <c r="P12" s="30">
         <f t="shared" ref="P12:P15" si="4">O12-L12</f>
-        <v>1.5651480682112584E-3</v>
+        <v>2.5633333333333064E-3</v>
       </c>
     </row>
     <row r="13" spans="2:16" x14ac:dyDescent="0.35">
@@ -1957,12 +1974,11 @@
         <v>1.3999999999999957E-2</v>
       </c>
       <c r="O13" s="37">
-        <f>'Check-calib2transprob'!L26</f>
-        <v>0.27846530823811355</v>
+        <v>0.28094999999999998</v>
       </c>
       <c r="P13" s="30">
         <f t="shared" si="4"/>
-        <v>-6.5346917618864242E-3</v>
+        <v>-4.049999999999998E-3</v>
       </c>
     </row>
     <row r="14" spans="2:16" x14ac:dyDescent="0.35">
@@ -2002,12 +2018,11 @@
         <v>-1.1577181208053733E-2</v>
       </c>
       <c r="O14" s="37">
-        <f>'Check-calib2transprob'!K26</f>
-        <v>0.39128197364604989</v>
+        <v>0.40410000000000001</v>
       </c>
       <c r="P14" s="30">
         <f t="shared" si="4"/>
-        <v>-1.4084514589640662E-4</v>
+        <v>1.2677181208053723E-2</v>
       </c>
     </row>
     <row r="15" spans="2:16" x14ac:dyDescent="0.35">
@@ -2045,12 +2060,11 @@
         <v>1.4577181208053694E-2</v>
       </c>
       <c r="O15" s="37">
-        <f>'Check-calib2transprob'!J26</f>
-        <v>7.3526698806152896E-2</v>
+        <v>6.2370000000000002E-2</v>
       </c>
       <c r="P15" s="30">
         <f t="shared" si="4"/>
-        <v>-1.7050482401900796E-2</v>
+        <v>-2.820718120805369E-2</v>
       </c>
     </row>
     <row r="16" spans="2:16" x14ac:dyDescent="0.35">
@@ -2085,11 +2099,11 @@
       </c>
       <c r="O16" s="3">
         <f t="shared" si="5"/>
-        <v>0.99999999999999978</v>
+        <v>1.0000099999999998</v>
       </c>
       <c r="P16" s="16">
         <f>ABS(P11)+ABS(P12)+ABS(P13)+ABS(P14)+ABS(P15)</f>
-        <v>4.7452038619367039E-2</v>
+        <v>6.4524362416107386E-2</v>
       </c>
     </row>
     <row r="17" spans="4:13" x14ac:dyDescent="0.35">
@@ -2097,7 +2111,7 @@
         <v>2</v>
       </c>
       <c r="M17" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="18" spans="4:13" x14ac:dyDescent="0.35">
@@ -2413,12 +2427,12 @@
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
   </sheetData>
@@ -2430,8 +2444,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98F466A6-35F3-4AB2-B6D8-919EDB7D04BD}">
   <dimension ref="A1:AE56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="Y4" sqref="Y4"/>
+    <sheetView tabSelected="1" topLeftCell="J2" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="Y12" sqref="Y12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -2442,20 +2456,20 @@
     <col min="6" max="6" width="8.75" customWidth="1"/>
     <col min="9" max="9" width="14.33203125" customWidth="1"/>
     <col min="10" max="15" width="11.1640625" customWidth="1"/>
-    <col min="18" max="18" width="14.33203125" customWidth="1"/>
-    <col min="19" max="23" width="11.1640625" customWidth="1"/>
+    <col min="18" max="18" width="14.33203125" hidden="1" customWidth="1"/>
+    <col min="19" max="23" width="11.1640625" hidden="1" customWidth="1"/>
     <col min="25" max="25" width="14.33203125" customWidth="1"/>
     <col min="26" max="31" width="11.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="3" spans="1:31" x14ac:dyDescent="0.35">
       <c r="S3" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="T3">
         <f>2/52</f>
@@ -2464,10 +2478,10 @@
     </row>
     <row r="4" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="Z4" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="AA4">
         <f>1/52</f>
@@ -2476,114 +2490,114 @@
     </row>
     <row r="5" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="6" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="7" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="10" spans="1:31" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A10" s="123" t="s">
+        <v>58</v>
+      </c>
+      <c r="B10" s="123"/>
+      <c r="C10" s="122" t="s">
+        <v>51</v>
+      </c>
+      <c r="D10" s="122"/>
+      <c r="E10" s="122"/>
+      <c r="F10" s="122"/>
+      <c r="I10" s="15" t="s">
+        <v>69</v>
+      </c>
+      <c r="J10" s="83" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="10" spans="1:31" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A10" s="105" t="s">
-        <v>59</v>
-      </c>
-      <c r="B10" s="105"/>
-      <c r="C10" s="104" t="s">
-        <v>52</v>
-      </c>
-      <c r="D10" s="104"/>
-      <c r="E10" s="104"/>
-      <c r="F10" s="104"/>
-      <c r="I10" s="15" t="s">
-        <v>70</v>
-      </c>
-      <c r="J10" s="83" t="s">
+      <c r="K10" s="83" t="s">
         <v>54</v>
-      </c>
-      <c r="K10" s="83" t="s">
-        <v>55</v>
       </c>
       <c r="L10" s="83" t="s">
         <v>14</v>
       </c>
       <c r="M10" s="83" t="s">
+        <v>55</v>
+      </c>
+      <c r="N10" s="83" t="s">
         <v>56</v>
       </c>
-      <c r="N10" s="83" t="s">
+      <c r="O10" s="84" t="s">
         <v>57</v>
       </c>
-      <c r="O10" s="84" t="s">
-        <v>58</v>
-      </c>
       <c r="P10" s="50"/>
-      <c r="R10" s="15" t="s">
-        <v>72</v>
+      <c r="R10" s="98" t="s">
+        <v>80</v>
       </c>
       <c r="S10" s="83" t="s">
+        <v>53</v>
+      </c>
+      <c r="T10" s="83" t="s">
         <v>54</v>
-      </c>
-      <c r="T10" s="83" t="s">
-        <v>55</v>
       </c>
       <c r="U10" s="83" t="s">
         <v>14</v>
       </c>
       <c r="V10" s="83" t="s">
+        <v>55</v>
+      </c>
+      <c r="W10" s="83" t="s">
         <v>56</v>
       </c>
-      <c r="W10" s="83" t="s">
-        <v>57</v>
-      </c>
       <c r="Y10" s="15" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="Z10" s="83" t="s">
+        <v>53</v>
+      </c>
+      <c r="AA10" s="83" t="s">
         <v>54</v>
-      </c>
-      <c r="AA10" s="83" t="s">
-        <v>55</v>
       </c>
       <c r="AB10" s="83" t="s">
         <v>14</v>
       </c>
       <c r="AC10" s="83" t="s">
+        <v>55</v>
+      </c>
+      <c r="AD10" s="83" t="s">
         <v>56</v>
       </c>
-      <c r="AD10" s="83" t="s">
-        <v>57</v>
-      </c>
-      <c r="AE10" s="84" t="s">
-        <v>58</v>
+      <c r="AE10" s="124" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="11" spans="1:31" ht="31" x14ac:dyDescent="0.35">
-      <c r="A11" s="105"/>
-      <c r="B11" s="105"/>
+      <c r="A11" s="123"/>
+      <c r="B11" s="123"/>
       <c r="C11" s="28" t="s">
+        <v>47</v>
+      </c>
+      <c r="D11" s="28" t="s">
         <v>48</v>
       </c>
-      <c r="D11" s="28" t="s">
+      <c r="E11" s="28" t="s">
         <v>49</v>
       </c>
-      <c r="E11" s="28" t="s">
+      <c r="F11" s="48" t="s">
         <v>50</v>
       </c>
-      <c r="F11" s="48" t="s">
-        <v>51</v>
-      </c>
       <c r="G11" s="75" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="I11" s="80" t="s">
-        <v>54</v>
-      </c>
-      <c r="J11" s="108">
+        <v>53</v>
+      </c>
+      <c r="J11" s="99">
         <f>1-SUM(K11:N11)</f>
         <v>0.43999999999999995</v>
       </c>
@@ -2605,49 +2619,49 @@
       </c>
       <c r="P11" s="36"/>
       <c r="R11" s="80" t="s">
-        <v>54</v>
-      </c>
-      <c r="S11" s="108">
+        <v>53</v>
+      </c>
+      <c r="S11" s="99">
         <f>-LN(1-J11)/$T$3</f>
         <v>15.075280876576493</v>
       </c>
-      <c r="T11" s="110">
+      <c r="T11" s="101">
         <f>-LN(1-K11)/$T$3</f>
         <v>15.543762019646129</v>
       </c>
-      <c r="U11" s="110">
+      <c r="U11" s="101">
         <f t="shared" ref="U11:U15" si="0">-LN(1-L11)/$T$3</f>
         <v>1.3336256540763149</v>
       </c>
-      <c r="V11" s="110">
+      <c r="V11" s="101">
         <f t="shared" ref="V11:V15" si="1">-LN(1-M11)/$T$3</f>
         <v>1.3336256540763149</v>
       </c>
-      <c r="W11" s="110">
+      <c r="W11" s="101">
         <f t="shared" ref="W11:W15" si="2">-LN(1-N11)/$T$3</f>
         <v>0.26130873219103767</v>
       </c>
       <c r="Y11" s="80" t="s">
-        <v>54</v>
-      </c>
-      <c r="Z11" s="115">
+        <v>53</v>
+      </c>
+      <c r="Z11" s="106">
         <f>1-SUM(AA11:AD11)</f>
         <v>0.68596615477797895</v>
       </c>
-      <c r="AA11" s="116">
+      <c r="AA11" s="107">
         <f t="shared" ref="AA11:AA15" si="3">1-EXP(-T11*$AA$4)</f>
         <v>0.25838015129043368</v>
       </c>
-      <c r="AB11" s="116">
+      <c r="AB11" s="107">
         <f t="shared" ref="AB11:AB15" si="4">1-EXP(-U11*$AA$4)</f>
         <v>2.5320565519103666E-2</v>
       </c>
-      <c r="AC11" s="116">
+      <c r="AC11" s="107">
         <f t="shared" ref="AC11:AC15" si="5">1-EXP(-V11*$AA$4)</f>
         <v>2.5320565519103666E-2</v>
       </c>
-      <c r="AD11" s="116">
-        <f t="shared" ref="AD11:AD15" si="6">1-EXP(-W11*$AA$4)</f>
+      <c r="AD11" s="107">
+        <f t="shared" ref="AD11:AD14" si="6">1-EXP(-W11*$AA$4)</f>
         <v>5.0125628933800348E-3</v>
       </c>
       <c r="AE11" s="55">
@@ -2656,11 +2670,11 @@
       </c>
     </row>
     <row r="12" spans="1:31" ht="29" x14ac:dyDescent="0.35">
-      <c r="A12" s="104" t="s">
+      <c r="A12" s="122" t="s">
+        <v>46</v>
+      </c>
+      <c r="B12" s="85" t="s">
         <v>47</v>
-      </c>
-      <c r="B12" s="85" t="s">
-        <v>48</v>
       </c>
       <c r="C12" s="93">
         <f>1-D12-E12</f>
@@ -2680,7 +2694,7 @@
         <v>1</v>
       </c>
       <c r="I12" s="80" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="J12" s="51">
         <v>0.05</v>
@@ -2704,48 +2718,48 @@
       </c>
       <c r="P12" s="36"/>
       <c r="R12" s="80" t="s">
-        <v>55</v>
-      </c>
-      <c r="S12" s="110">
+        <v>54</v>
+      </c>
+      <c r="S12" s="101">
         <f>-LN(1-J12)/$T$3</f>
         <v>1.3336256540763149</v>
       </c>
-      <c r="T12" s="108">
+      <c r="T12" s="99">
         <f>-LN(1-K12)/$T$3</f>
         <v>25.850559106940537</v>
       </c>
-      <c r="U12" s="110">
+      <c r="U12" s="101">
         <f t="shared" si="0"/>
         <v>4.2254921669421481</v>
       </c>
-      <c r="V12" s="110">
+      <c r="V12" s="101">
         <f t="shared" si="1"/>
         <v>4.2254921669421481</v>
       </c>
-      <c r="W12" s="110">
+      <c r="W12" s="101">
         <f t="shared" si="2"/>
         <v>0.52527039025550604</v>
       </c>
       <c r="Y12" s="80" t="s">
-        <v>55</v>
-      </c>
-      <c r="Z12" s="116">
+        <v>54</v>
+      </c>
+      <c r="Z12" s="107">
         <f t="shared" ref="Z12:Z15" si="7">1-EXP(-S12*$AA$4)</f>
         <v>2.5320565519103666E-2</v>
       </c>
-      <c r="AA12" s="115">
+      <c r="AA12" s="106">
         <f>1-SUM(Z12,AB12:AD12)</f>
         <v>0.80853781960064042</v>
       </c>
-      <c r="AB12" s="116">
+      <c r="AB12" s="107">
         <f t="shared" si="4"/>
         <v>7.8045554270711248E-2</v>
       </c>
-      <c r="AC12" s="116">
+      <c r="AC12" s="107">
         <f t="shared" si="5"/>
         <v>7.8045554270711248E-2</v>
       </c>
-      <c r="AD12" s="116">
+      <c r="AD12" s="107">
         <f t="shared" si="6"/>
         <v>1.005050633883342E-2</v>
       </c>
@@ -2755,9 +2769,9 @@
       </c>
     </row>
     <row r="13" spans="1:31" ht="31" x14ac:dyDescent="0.35">
-      <c r="A13" s="104"/>
+      <c r="A13" s="122"/>
       <c r="B13" s="87" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C13" s="88">
         <f>1-D13-E13</f>
@@ -2803,46 +2817,46 @@
       <c r="R13" s="81" t="s">
         <v>14</v>
       </c>
-      <c r="S13" s="111">
+      <c r="S13" s="102">
         <f t="shared" ref="S13:S15" si="9">-LN(1-J13)/$T$3</f>
         <v>1.3336256540763149</v>
       </c>
-      <c r="T13" s="111">
+      <c r="T13" s="102">
         <f t="shared" ref="T13:T15" si="10">-LN(1-K13)/$T$3</f>
         <v>7.4797338837463032</v>
       </c>
-      <c r="U13" s="112">
+      <c r="U13" s="103">
         <f t="shared" si="0"/>
         <v>18.547097084814084</v>
       </c>
-      <c r="V13" s="111">
+      <c r="V13" s="102">
         <f t="shared" si="1"/>
         <v>4.2254921669421481</v>
       </c>
-      <c r="W13" s="111">
+      <c r="W13" s="102">
         <f t="shared" si="2"/>
         <v>1.0613718575266342</v>
       </c>
       <c r="Y13" s="81" t="s">
         <v>14</v>
       </c>
-      <c r="Z13" s="117">
+      <c r="Z13" s="108">
         <f t="shared" si="7"/>
         <v>2.5320565519103666E-2</v>
       </c>
-      <c r="AA13" s="117">
+      <c r="AA13" s="108">
         <f t="shared" si="3"/>
         <v>0.13397459621556129</v>
       </c>
-      <c r="AB13" s="118">
+      <c r="AB13" s="109">
         <f>1-SUM(Z13:AA13,AC13:AD13)</f>
         <v>0.74245518110789499</v>
       </c>
-      <c r="AC13" s="117">
+      <c r="AC13" s="108">
         <f t="shared" si="5"/>
         <v>7.8045554270711248E-2</v>
       </c>
-      <c r="AD13" s="117">
+      <c r="AD13" s="108">
         <f t="shared" si="6"/>
         <v>2.0204102886728803E-2</v>
       </c>
@@ -2852,9 +2866,9 @@
       </c>
     </row>
     <row r="14" spans="1:31" ht="29" x14ac:dyDescent="0.35">
-      <c r="A14" s="104"/>
+      <c r="A14" s="122"/>
       <c r="B14" s="90" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C14" s="91">
         <f>1-D14-E14</f>
@@ -2874,7 +2888,7 @@
         <v>1</v>
       </c>
       <c r="I14" s="82" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="J14" s="54">
         <v>0.03</v>
@@ -2897,48 +2911,48 @@
         <v>0.191</v>
       </c>
       <c r="R14" s="82" t="s">
-        <v>56</v>
-      </c>
-      <c r="S14" s="113">
+        <v>55</v>
+      </c>
+      <c r="S14" s="104">
         <f t="shared" si="9"/>
         <v>0.79193939460242291</v>
       </c>
-      <c r="T14" s="113">
+      <c r="T14" s="104">
         <f t="shared" si="10"/>
         <v>5.8017323341694524</v>
       </c>
-      <c r="U14" s="113">
+      <c r="U14" s="104">
         <f t="shared" si="0"/>
         <v>9.2735485424070436</v>
       </c>
-      <c r="V14" s="114">
+      <c r="V14" s="105">
         <f t="shared" si="1"/>
         <v>12.851704367184283</v>
       </c>
-      <c r="W14" s="113">
+      <c r="W14" s="104">
         <f t="shared" si="2"/>
         <v>2.1679218324153262</v>
       </c>
       <c r="Y14" s="82" t="s">
-        <v>56</v>
-      </c>
-      <c r="Z14" s="119">
+        <v>55</v>
+      </c>
+      <c r="Z14" s="110">
         <f t="shared" si="7"/>
         <v>1.5114219820389518E-2</v>
       </c>
-      <c r="AA14" s="119">
+      <c r="AA14" s="110">
         <f t="shared" si="3"/>
         <v>0.10557280900008414</v>
       </c>
-      <c r="AB14" s="119">
+      <c r="AB14" s="110">
         <f t="shared" si="4"/>
         <v>0.16333997346592444</v>
       </c>
-      <c r="AC14" s="120">
+      <c r="AC14" s="111">
         <f>1-SUM(Z14:AB14,AD14)</f>
         <v>0.67513930237614583</v>
       </c>
-      <c r="AD14" s="119">
+      <c r="AD14" s="110">
         <f t="shared" si="6"/>
         <v>4.0833695337456066E-2</v>
       </c>
@@ -2955,7 +2969,7 @@
       <c r="E15" s="28"/>
       <c r="F15" s="48"/>
       <c r="I15" s="82" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="J15" s="54">
         <v>0.03</v>
@@ -2978,48 +2992,48 @@
         <v>5.8999999999999997E-2</v>
       </c>
       <c r="R15" s="82" t="s">
-        <v>57</v>
-      </c>
-      <c r="S15" s="113">
+        <v>56</v>
+      </c>
+      <c r="S15" s="104">
         <f t="shared" si="9"/>
         <v>0.79193939460242291</v>
       </c>
-      <c r="T15" s="113">
+      <c r="T15" s="104">
         <f t="shared" si="10"/>
         <v>1.3336256540763149</v>
       </c>
-      <c r="U15" s="113">
+      <c r="U15" s="104">
         <f t="shared" si="0"/>
         <v>7.4797338837463032</v>
       </c>
-      <c r="V15" s="113">
+      <c r="V15" s="104">
         <f t="shared" si="1"/>
         <v>7.4797338837463032</v>
       </c>
-      <c r="W15" s="114">
+      <c r="W15" s="105">
         <f t="shared" si="2"/>
         <v>14.162906561483469</v>
       </c>
       <c r="Y15" s="82" t="s">
-        <v>57</v>
-      </c>
-      <c r="Z15" s="119">
+        <v>56</v>
+      </c>
+      <c r="Z15" s="110">
         <f t="shared" si="7"/>
         <v>1.5114219820389518E-2</v>
       </c>
-      <c r="AA15" s="119">
+      <c r="AA15" s="110">
         <f t="shared" si="3"/>
         <v>2.5320565519103666E-2</v>
       </c>
-      <c r="AB15" s="119">
+      <c r="AB15" s="110">
         <f t="shared" si="4"/>
         <v>0.13397459621556129</v>
       </c>
-      <c r="AC15" s="119">
+      <c r="AC15" s="110">
         <f t="shared" si="5"/>
         <v>0.13397459621556129</v>
       </c>
-      <c r="AD15" s="120">
+      <c r="AD15" s="111">
         <f>1-SUM(Z15:AC15)</f>
         <v>0.69161602222938423</v>
       </c>
@@ -3058,7 +3072,7 @@
     </row>
     <row r="17" spans="1:31" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A17" s="67" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B17" s="68"/>
       <c r="C17" s="68" t="str">
@@ -3074,11 +3088,11 @@
         <v>Uncontrolled</v>
       </c>
       <c r="F17" s="67" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G17" s="68"/>
       <c r="H17" s="64" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="I17" s="63"/>
       <c r="J17" s="63" t="str">
@@ -3102,7 +3116,7 @@
         <v>5 - Not controlled at all</v>
       </c>
       <c r="O17" s="67" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="Q17" s="66"/>
       <c r="R17" s="96"/>
@@ -3112,7 +3126,7 @@
       <c r="V17" s="96"/>
       <c r="W17" s="96"/>
       <c r="X17" s="64" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="Y17" s="96"/>
       <c r="Z17" s="96" t="str">
@@ -3136,7 +3150,7 @@
         <v>5 - Not controlled at all</v>
       </c>
       <c r="AE17" s="67" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="18" spans="1:31" x14ac:dyDescent="0.35">
@@ -3144,7 +3158,7 @@
         <v>0</v>
       </c>
       <c r="B18" s="68" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C18" s="94">
         <v>0</v>
@@ -3164,7 +3178,7 @@
         <v>0</v>
       </c>
       <c r="I18" s="63" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="J18" s="37">
         <v>0</v>
@@ -3187,16 +3201,16 @@
       </c>
       <c r="Q18" s="66"/>
       <c r="R18" s="96"/>
-      <c r="S18" s="109"/>
+      <c r="S18" s="100"/>
       <c r="T18" s="79"/>
       <c r="U18" s="79"/>
       <c r="V18" s="79"/>
-      <c r="W18" s="109"/>
+      <c r="W18" s="100"/>
       <c r="X18" s="77">
         <v>0</v>
       </c>
       <c r="Y18" s="96" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="Z18" s="37">
         <v>0</v>
@@ -3223,7 +3237,7 @@
         <v>1</v>
       </c>
       <c r="B19" s="68" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C19" s="61">
         <f>$C18*C$12 + $D18*C$13 + $E18*C$14</f>
@@ -3246,7 +3260,7 @@
         <v>1</v>
       </c>
       <c r="I19" s="63" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="J19" s="36">
         <f>$J18*J$11 + $K18*J$12 + $L18*J$13 + $M18*J$14 + $N18*J$15</f>
@@ -3274,16 +3288,16 @@
       </c>
       <c r="P19" s="62"/>
       <c r="R19" s="96"/>
-      <c r="S19" s="109"/>
-      <c r="T19" s="109"/>
-      <c r="U19" s="109"/>
-      <c r="V19" s="109"/>
-      <c r="W19" s="109"/>
+      <c r="S19" s="100"/>
+      <c r="T19" s="100"/>
+      <c r="U19" s="100"/>
+      <c r="V19" s="100"/>
+      <c r="W19" s="100"/>
       <c r="X19" s="78">
         <v>1</v>
       </c>
       <c r="Y19" s="96" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="Z19" s="36">
         <f>$Z18*Z$11 + $AA18*Z$12 + $AB18*Z$13 + $AC18*Z$14 + $AD18*Z$15</f>
@@ -3315,7 +3329,7 @@
         <v>2</v>
       </c>
       <c r="B20" s="69" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C20" s="79">
         <f t="shared" ref="C20:C48" si="20">$C19*C$12 + $D19*C$13 + $E19*C$14</f>
@@ -3338,7 +3352,7 @@
         <v>2</v>
       </c>
       <c r="I20" s="69" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="J20" s="36">
         <f>$J19*J$11 + $K19*J$12 + $L19*J$13 + $M19*J$14 + $N19*J$15</f>
@@ -3375,7 +3389,7 @@
         <v>2</v>
       </c>
       <c r="Y20" s="69" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="Z20" s="36">
         <f t="shared" ref="Z20:Z48" si="27">$Z19*Z$11 + $AA19*Z$12 + $AB19*Z$13 + $AC19*Z$14 + $AD19*Z$15</f>
@@ -3407,7 +3421,7 @@
         <v>3</v>
       </c>
       <c r="B21" s="68" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C21" s="61">
         <f t="shared" si="20"/>
@@ -3430,7 +3444,7 @@
         <v>3</v>
       </c>
       <c r="I21" s="69" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J21" s="36">
         <f t="shared" ref="J21:J48" si="32">$J20*J$11 + $K20*J$12 + $L20*J$13 + $M20*J$14 + $N20*J$15</f>
@@ -3467,7 +3481,7 @@
         <v>3</v>
       </c>
       <c r="Y21" s="96" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="Z21" s="36">
         <f t="shared" si="27"/>
@@ -3499,7 +3513,7 @@
         <v>4</v>
       </c>
       <c r="B22" s="68" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C22" s="61">
         <f t="shared" si="20"/>
@@ -3522,7 +3536,7 @@
         <v>4</v>
       </c>
       <c r="I22" s="69" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="J22" s="36">
         <f t="shared" si="32"/>
@@ -3558,7 +3572,7 @@
         <v>4</v>
       </c>
       <c r="Y22" s="96" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="Z22" s="36">
         <f t="shared" si="27"/>
@@ -3643,7 +3657,7 @@
         <v>5</v>
       </c>
       <c r="Y23" s="96" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="Z23" s="36">
         <f t="shared" si="27"/>
@@ -5674,49 +5688,49 @@
     </row>
     <row r="52" spans="9:31" x14ac:dyDescent="0.35">
       <c r="I52" s="69" t="s">
-        <v>64</v>
-      </c>
-      <c r="J52" s="106">
+        <v>63</v>
+      </c>
+      <c r="J52" s="120">
         <f>J48+K48</f>
         <v>0.46505834936992835</v>
       </c>
-      <c r="K52" s="106"/>
+      <c r="K52" s="120"/>
       <c r="L52" s="36">
         <f>L48</f>
         <v>0.27827636738401695</v>
       </c>
-      <c r="M52" s="106">
+      <c r="M52" s="120">
         <f>M48+N48</f>
         <v>0.25666528324605486</v>
       </c>
-      <c r="N52" s="106"/>
+      <c r="N52" s="120"/>
       <c r="O52" s="61">
         <f>SUM(J52:N52)</f>
         <v>1</v>
       </c>
       <c r="R52" s="69"/>
-      <c r="S52" s="106"/>
-      <c r="T52" s="106"/>
+      <c r="S52" s="120"/>
+      <c r="T52" s="120"/>
       <c r="U52" s="36"/>
-      <c r="V52" s="106"/>
-      <c r="W52" s="106"/>
+      <c r="V52" s="120"/>
+      <c r="W52" s="120"/>
       <c r="Y52" s="69" t="s">
-        <v>64</v>
-      </c>
-      <c r="Z52" s="106">
+        <v>63</v>
+      </c>
+      <c r="Z52" s="120">
         <f>Z48+AA48</f>
         <v>0.46812446329601987</v>
       </c>
-      <c r="AA52" s="106"/>
+      <c r="AA52" s="120"/>
       <c r="AB52" s="36">
         <f>AB48</f>
         <v>0.28076632247765299</v>
       </c>
-      <c r="AC52" s="106">
+      <c r="AC52" s="120">
         <f>AC48+AD48</f>
         <v>0.25110921422632748</v>
       </c>
-      <c r="AD52" s="106"/>
+      <c r="AD52" s="120"/>
       <c r="AE52" s="61">
         <f>SUM(Z52:AD52)</f>
         <v>1.0000000000000004</v>
@@ -5724,75 +5738,75 @@
     </row>
     <row r="54" spans="9:31" x14ac:dyDescent="0.35">
       <c r="I54" s="72" t="s">
-        <v>37</v>
-      </c>
-      <c r="J54" s="107">
+        <v>36</v>
+      </c>
+      <c r="J54" s="121">
         <f>ABS(J52-C36)</f>
         <v>0.28069545903540727</v>
       </c>
-      <c r="K54" s="107"/>
+      <c r="K54" s="121"/>
       <c r="L54" s="73">
         <f>ABS(L52-D36)</f>
         <v>7.450292497591432E-2</v>
       </c>
-      <c r="M54" s="107">
+      <c r="M54" s="121">
         <f>ABS(M52-E36)</f>
         <v>0.20619253405949267</v>
       </c>
-      <c r="N54" s="107"/>
+      <c r="N54" s="121"/>
       <c r="O54" s="74">
         <f>SUM(J54:N54)</f>
         <v>0.56139091807081432</v>
       </c>
       <c r="R54" s="72"/>
-      <c r="S54" s="107"/>
-      <c r="T54" s="107"/>
+      <c r="S54" s="121"/>
+      <c r="T54" s="121"/>
       <c r="U54" s="97"/>
-      <c r="V54" s="107"/>
-      <c r="W54" s="107"/>
+      <c r="V54" s="121"/>
+      <c r="W54" s="121"/>
       <c r="Y54" s="72" t="s">
-        <v>77</v>
-      </c>
-      <c r="Z54" s="107">
+        <v>73</v>
+      </c>
+      <c r="Z54" s="121">
         <f>ABS(Z52-J52)</f>
         <v>3.0661139260915182E-3</v>
       </c>
-      <c r="AA54" s="107"/>
+      <c r="AA54" s="121"/>
       <c r="AB54" s="97">
         <f>ABS(AB52-L52)</f>
         <v>2.4899550936360315E-3</v>
       </c>
-      <c r="AC54" s="107">
+      <c r="AC54" s="121">
         <f>ABS(AC52-M52)</f>
         <v>5.5560690197273832E-3</v>
       </c>
-      <c r="AD54" s="107"/>
+      <c r="AD54" s="121"/>
       <c r="AE54" s="74">
         <f>SUM(Z54:AD54)</f>
         <v>1.1112138039454933E-2</v>
       </c>
     </row>
     <row r="55" spans="9:31" x14ac:dyDescent="0.35">
-      <c r="Y55" s="121" t="s">
-        <v>78</v>
-      </c>
-      <c r="Z55" s="122">
+      <c r="Y55" s="112" t="s">
+        <v>74</v>
+      </c>
+      <c r="Z55" s="113">
         <f>ABS(Z48-AE11)</f>
         <v>8.9385601660808556E-3</v>
       </c>
-      <c r="AA55" s="122">
+      <c r="AA55" s="113">
         <f>ABS(AA48-AE12)</f>
         <v>1.9369765378993153E-3</v>
       </c>
-      <c r="AB55" s="122">
+      <c r="AB55" s="113">
         <f>ABS(AB48-AE13)</f>
         <v>9.7663224776529667E-3</v>
       </c>
-      <c r="AC55" s="122">
+      <c r="AC55" s="113">
         <f>ABS(AC48-AE14)</f>
         <v>1.9976236898767152E-3</v>
       </c>
-      <c r="AD55" s="122">
+      <c r="AD55" s="113">
         <f>ABS(AD48-AE15)</f>
         <v>8.8840946354924732E-4</v>
       </c>
@@ -5802,14 +5816,21 @@
       </c>
     </row>
     <row r="56" spans="9:31" x14ac:dyDescent="0.35">
-      <c r="Z56" s="122"/>
-      <c r="AA56" s="122"/>
-      <c r="AB56" s="122"/>
-      <c r="AC56" s="122"/>
-      <c r="AD56" s="122"/>
+      <c r="Z56" s="113"/>
+      <c r="AA56" s="113"/>
+      <c r="AB56" s="113"/>
+      <c r="AC56" s="113"/>
+      <c r="AD56" s="113"/>
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="A12:A14"/>
+    <mergeCell ref="A10:B11"/>
+    <mergeCell ref="J52:K52"/>
+    <mergeCell ref="M52:N52"/>
+    <mergeCell ref="J54:K54"/>
+    <mergeCell ref="M54:N54"/>
+    <mergeCell ref="C10:F10"/>
     <mergeCell ref="AC52:AD52"/>
     <mergeCell ref="Z54:AA54"/>
     <mergeCell ref="AC54:AD54"/>
@@ -5818,13 +5839,6 @@
     <mergeCell ref="S54:T54"/>
     <mergeCell ref="V54:W54"/>
     <mergeCell ref="Z52:AA52"/>
-    <mergeCell ref="A12:A14"/>
-    <mergeCell ref="A10:B11"/>
-    <mergeCell ref="J52:K52"/>
-    <mergeCell ref="M52:N52"/>
-    <mergeCell ref="J54:K54"/>
-    <mergeCell ref="M54:N54"/>
-    <mergeCell ref="C10:F10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>

</xml_diff>